<commit_message>
fixed CFG (added 23), fixed evry branch, and multiple condition
</commit_message>
<xml_diff>
--- a/evry branch.xlsx
+++ b/evry branch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FINKI\4 semestar\sovtversko inzinerstvo\SI_2023_lab2_213202\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D24378-E97B-4651-9B1F-32F43C36E133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017BCF3A-CE59-4930-95CC-A8072D1EBFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F6B1A9E9-619B-4CD3-919B-E92EC71CACBA}"/>
   </bookViews>
@@ -137,19 +137,19 @@
     <t>19.3-19.2</t>
   </si>
   <si>
-    <t>password.lengt=7 username=null (@) list.size&gt;5</t>
-  </si>
-  <si>
-    <t>passwrod.length&gt;8 &amp;&amp; password!=username &amp;&amp; username!=null &amp;&amp; email nema @  password=s123s123</t>
-  </si>
-  <si>
-    <t>password = s123+s123</t>
-  </si>
-  <si>
-    <t>password=s123 s123</t>
-  </si>
-  <si>
     <t>usser==null</t>
+  </si>
+  <si>
+    <t>user4=new User("Mahmud" , "s12     s123","memedoskim16@gmail.com") // space vo password</t>
+  </si>
+  <si>
+    <t>user3=new User("Mahmud" , "s123++s123","memedoskim16@gmail.com")//specail charcter in password</t>
+  </si>
+  <si>
+    <t>user2=new User("Mahmud" , "s123s123","mahmud.com")// no @ In email</t>
+  </si>
+  <si>
+    <t>user1=new User(null,"s123","aaa@test.com") // username = null</t>
   </si>
 </sst>
 </file>
@@ -187,9 +187,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -509,15 +511,15 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.77734375" customWidth="1"/>
     <col min="3" max="3" width="37.44140625" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -525,20 +527,20 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -550,7 +552,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -561,15 +563,16 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5">
@@ -577,7 +580,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -585,7 +588,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -596,7 +599,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -604,7 +607,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9">
@@ -612,7 +615,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
@@ -620,7 +623,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -628,7 +631,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -636,7 +639,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -644,7 +647,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -652,7 +655,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -660,7 +663,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -668,7 +671,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -676,7 +679,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -684,7 +687,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -692,7 +695,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -700,7 +703,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -708,7 +711,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -719,7 +722,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23">
@@ -727,7 +730,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C24">
@@ -735,7 +738,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C25">
@@ -746,7 +749,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C26">
@@ -757,7 +760,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E27">
@@ -765,7 +768,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C28">
@@ -776,7 +779,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C29">
@@ -787,7 +790,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C30">
@@ -798,7 +801,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D31">
@@ -806,7 +809,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C32">
@@ -817,7 +820,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C33">
@@ -828,7 +831,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
+      <c r="A34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>